<commit_message>
fix save grap and train process
</commit_message>
<xml_diff>
--- a/output/out_excel/data_M2.xlsx
+++ b/output/out_excel/data_M2.xlsx
@@ -470,22 +470,22 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1.014331659549823</v>
+        <v>1.525965269531893</v>
       </c>
       <c r="C2" t="n">
-        <v>1.050285272452345</v>
+        <v>1.322619210585525</v>
       </c>
       <c r="D2" t="n">
-        <v>1.059882760245282</v>
+        <v>1.169002513005085</v>
       </c>
       <c r="E2" t="n">
-        <v>1.054868554047321</v>
+        <v>1.220884036319589</v>
       </c>
       <c r="F2" t="n">
-        <v>1.061255527042197</v>
+        <v>1.332915022613899</v>
       </c>
       <c r="G2" t="n">
-        <v>1.048124754667394</v>
+        <v>1.314277210411198</v>
       </c>
     </row>
     <row r="3">
@@ -493,22 +493,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>1.012911344296523</v>
+        <v>1.539836047058403</v>
       </c>
       <c r="C3" t="n">
-        <v>1.065518798767686</v>
+        <v>1.24644318523582</v>
       </c>
       <c r="D3" t="n">
-        <v>1.025624351429833</v>
+        <v>1.236655072989541</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9457389154152427</v>
+        <v>1.202193997384603</v>
       </c>
       <c r="F3" t="n">
-        <v>1.054860830806526</v>
+        <v>1.189771017454148</v>
       </c>
       <c r="G3" t="n">
-        <v>1.020930848143162</v>
+        <v>1.282979864024503</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>1.015771754997067</v>
+        <v>1.41628701880448</v>
       </c>
       <c r="C4" t="n">
-        <v>1.027469948605009</v>
+        <v>1.060330398414768</v>
       </c>
       <c r="D4" t="n">
-        <v>1.018717197407606</v>
+        <v>1.269980323660571</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9971558945237022</v>
+        <v>1.239977132725892</v>
       </c>
       <c r="F4" t="n">
-        <v>1.021557016426263</v>
+        <v>1.294330520127511</v>
       </c>
       <c r="G4" t="n">
-        <v>1.016134362391929</v>
+        <v>1.256181078746645</v>
       </c>
     </row>
     <row r="5">
@@ -539,22 +539,22 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6450925924857041</v>
+        <v>1.54346131258994</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8258425826688109</v>
+        <v>1.175073221374955</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7777624834713202</v>
+        <v>0.978708444294902</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8269744661499486</v>
+        <v>0.9916108842675304</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7245899375936746</v>
+        <v>1.14343627414154</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7600524124738917</v>
+        <v>1.166458027333773</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4344392576103301</v>
+        <v>0.9240847822018921</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5482061419293882</v>
+        <v>0.7970027915421876</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4394049117143036</v>
+        <v>0.5682791430575371</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4909539906644234</v>
+        <v>0.5827491581979505</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4445059723996115</v>
+        <v>0.707176145132798</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4715020548636114</v>
+        <v>0.7158584040264729</v>
       </c>
     </row>
     <row r="7">
@@ -585,22 +585,22 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2171221067738823</v>
+        <v>0.3957573216720039</v>
       </c>
       <c r="C7" t="n">
-        <v>0.330406139584047</v>
+        <v>0.5660907733492631</v>
       </c>
       <c r="D7" t="n">
-        <v>0.242248734407065</v>
+        <v>0.3794973895153716</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2703968348095198</v>
+        <v>0.3192274030934538</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2257784573396238</v>
+        <v>0.4301859734429974</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2571904545828275</v>
+        <v>0.4181517722146179</v>
       </c>
     </row>
     <row r="8">
@@ -608,22 +608,22 @@
         <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1612630610290465</v>
+        <v>0.3760537054939977</v>
       </c>
       <c r="C8" t="n">
-        <v>0.219555217738983</v>
+        <v>0.3420546008335217</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1482195845859692</v>
+        <v>0.1578135723174616</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1325751857841843</v>
+        <v>0.1412350080299828</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1195469176456914</v>
+        <v>0.2201480844511626</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1562319933567749</v>
+        <v>0.2474609942252253</v>
       </c>
     </row>
     <row r="9">
@@ -631,22 +631,22 @@
         <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2266564107880261</v>
+        <v>0.7108270233441099</v>
       </c>
       <c r="C9" t="n">
-        <v>0.201505826968214</v>
+        <v>0.2090492859052139</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1236450440497338</v>
+        <v>0.09728488920783651</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07708377356006002</v>
+        <v>0.09087548139238655</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0881620391499558</v>
+        <v>0.1282813427818635</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1434106189031979</v>
+        <v>0.2472636045262821</v>
       </c>
     </row>
     <row r="10">
@@ -654,22 +654,22 @@
         <v>45</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8115402389216471</v>
+        <v>0.9788722036769728</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2631031521768847</v>
+        <v>0.2096266312732893</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1465371511494645</v>
+        <v>0.09393413116731208</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0680638443749465</v>
+        <v>0.05070654976853972</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08919867328889552</v>
+        <v>0.1487939289094512</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2756886119823676</v>
+        <v>0.296386688959113</v>
       </c>
     </row>
     <row r="11">
@@ -677,22 +677,22 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8406393229204994</v>
+        <v>1.899489556631275</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2978895587637934</v>
+        <v>0.1982595958728413</v>
       </c>
       <c r="D11" t="n">
-        <v>0.167547109623763</v>
+        <v>0.1169534596228009</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06878595847428326</v>
+        <v>0.04180567673729096</v>
       </c>
       <c r="F11" t="n">
-        <v>0.09082377738341374</v>
+        <v>0.1259859422456563</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2931371454331505</v>
+        <v>0.4764988462219729</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>55</v>
       </c>
       <c r="B12" t="n">
-        <v>1.242183803313677</v>
+        <v>1.536941295366478</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3200276998293393</v>
+        <v>0.1932361358617809</v>
       </c>
       <c r="D12" t="n">
-        <v>0.161116142196846</v>
+        <v>0.1370453144309562</v>
       </c>
       <c r="E12" t="n">
-        <v>0.06598491196163647</v>
+        <v>0.04742613787190875</v>
       </c>
       <c r="F12" t="n">
-        <v>0.09864242101955023</v>
+        <v>0.1408756989364836</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3775909956642099</v>
+        <v>0.4111049164935216</v>
       </c>
     </row>
     <row r="13">
@@ -723,22 +723,22 @@
         <v>60</v>
       </c>
       <c r="B13" t="n">
-        <v>1.332598597770007</v>
+        <v>2.149965669878457</v>
       </c>
       <c r="C13" t="n">
-        <v>0.336220184005617</v>
+        <v>0.2020063127782311</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1671268948457963</v>
+        <v>0.1422063693269555</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07176426169076</v>
+        <v>0.05611950484942585</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1058256696609025</v>
+        <v>0.1479585045290324</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4027071215946166</v>
+        <v>0.5396512722724205</v>
       </c>
     </row>
     <row r="14">
@@ -746,22 +746,22 @@
         <v>65</v>
       </c>
       <c r="B14" t="n">
-        <v>1.363241917770394</v>
+        <v>1.558743048855251</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3415222652753718</v>
+        <v>0.2059833804856536</v>
       </c>
       <c r="D14" t="n">
-        <v>0.180570211920861</v>
+        <v>0.1547725216578992</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07495682775108348</v>
+        <v>0.06183024005044346</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1098729885030374</v>
+        <v>0.1481775129269887</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4140328422441495</v>
+        <v>0.4259013407952471</v>
       </c>
     </row>
     <row r="15">
@@ -769,22 +769,22 @@
         <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>1.398939725562193</v>
+        <v>1.853629939407736</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3477939658289699</v>
+        <v>0.2053231409355986</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1827876344952184</v>
+        <v>0.1677313618360533</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0752686309339714</v>
+        <v>0.0599667715278106</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1134031799548323</v>
+        <v>0.1477482588111194</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4236386273550371</v>
+        <v>0.4868798945036635</v>
       </c>
     </row>
     <row r="16">
@@ -792,22 +792,22 @@
         <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>1.410871107756642</v>
+        <v>1.789704015869725</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3500461805791129</v>
+        <v>0.2048315381960227</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1851770522126881</v>
+        <v>0.1694420174567767</v>
       </c>
       <c r="E16" t="n">
-        <v>0.07563994690488696</v>
+        <v>0.06445625548496803</v>
       </c>
       <c r="F16" t="n">
-        <v>0.115399027519312</v>
+        <v>0.1502687465957444</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4274266629945284</v>
+        <v>0.4757405147206473</v>
       </c>
     </row>
     <row r="17">
@@ -815,22 +815,22 @@
         <v>80</v>
       </c>
       <c r="B17" t="n">
-        <v>1.408250252691499</v>
+        <v>1.801132914686453</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3506571450688694</v>
+        <v>0.2050245889580702</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1866156640811529</v>
+        <v>0.171955657599162</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07713039777647523</v>
+        <v>0.06326199470326921</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1155213346704279</v>
+        <v>0.151041449405909</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4276349588576848</v>
+        <v>0.4784833210705727</v>
       </c>
     </row>
     <row r="18">
@@ -838,22 +838,22 @@
         <v>85</v>
       </c>
       <c r="B18" t="n">
-        <v>1.41570749338034</v>
+        <v>1.799097682926146</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3513036612779046</v>
+        <v>0.2053059878068844</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1875254822273187</v>
+        <v>0.1720745515957336</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07667567735413139</v>
+        <v>0.06356284793215772</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1165799358474671</v>
+        <v>0.1508856369303</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4295584500174325</v>
+        <v>0.4781853414382443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>